<commit_message>
Update 3/19: CDC remove the 333 number
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ohio_CDC" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Negative PUIs</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Delaware</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +719,20 @@
         <v>333</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43909</v>
+      </c>
+      <c r="B15">
+        <v>116</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -721,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +752,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -793,80 +813,86 @@
       <c r="T1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
-      <c r="U2">
-        <f>SUM(B2:T2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W2">
+        <f>SUM(B2:V2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U14" si="0">SUM(B3:T3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W3">
+        <f t="shared" ref="W3:W15" si="0">SUM(B3:V3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -885,12 +911,12 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -915,12 +941,12 @@
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -945,12 +971,12 @@
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -966,12 +992,12 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -1005,12 +1031,12 @@
       <c r="R13">
         <v>1</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1041,91 +1067,132 @@
       <c r="T14">
         <v>1</v>
       </c>
-      <c r="U14">
+      <c r="W14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43909</v>
+      </c>
       <c r="B15">
-        <f>SUM(B2:B14)</f>
-        <v>38</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:U15" si="1">SUM(C2:C14)</f>
-        <v>3</v>
-      </c>
-      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" ref="B16:S16" si="1">SUM(B2:B15)</f>
+        <v>53</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F15">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I15">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J15">
+      <c r="H16">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N15">
+      <c r="L16">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="Q16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="T15">
+      <c r="R16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="U15">
+      <c r="S16">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <f>SUM(T2:T15)</f>
+        <v>2</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ref="U16" si="2">SUM(U2:U15)</f>
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ref="V16" si="3">SUM(V2:V15)</f>
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16" si="4">SUM(W2:W15)</f>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fit_logistic and save pictures. Also update ridership data for 3/25
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Ohio_CDC" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Negative PUIs</t>
   </si>
@@ -186,13 +186,52 @@
   </si>
   <si>
     <t>Licking</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>Columbiana</t>
+  </si>
+  <si>
+    <t>Greene</t>
+  </si>
+  <si>
+    <t>Hancock</t>
+  </si>
+  <si>
+    <t>Portage</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Sandusky</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Highland</t>
+  </si>
+  <si>
+    <t>Knox</t>
+  </si>
+  <si>
+    <t>Madison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +373,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4A4A4A"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -677,7 +722,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -687,6 +732,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1008,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,6 +1350,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B18">
+        <v>351</v>
+      </c>
+      <c r="E18">
+        <v>83</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B19">
+        <v>442</v>
+      </c>
+      <c r="E19">
+        <v>104</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1312,18 +1386,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI18"/>
+  <dimension ref="A1:AV22"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="48" max="48" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1340,166 +1415,205 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AE1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AG1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AH1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AI1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AJ1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AK1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AM1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" t="s">
         <v>6</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AO1" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AP1" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AQ1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AR1" t="s">
         <v>46</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AS1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AT1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
-      <c r="AI2">
-        <f>SUM(B2:AH2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AV2">
+        <f t="shared" ref="AV2:AV19" si="0">SUM(B2:AU2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
-      <c r="AI3">
-        <f t="shared" ref="AI3:AI15" si="0">SUM(B3:AH3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AV3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
-      <c r="AI4">
+      <c r="AV4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="AI5">
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="AV5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
-      <c r="AI6">
+      <c r="AV6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
-      <c r="AC7">
-        <v>1</v>
-      </c>
-      <c r="AI7">
+      <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AV7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AI8">
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -1509,141 +1623,141 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="AC9">
-        <v>1</v>
-      </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
-      <c r="AI9">
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AV9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>5</v>
       </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="U10">
+      <c r="Q10">
         <v>1</v>
       </c>
       <c r="AC10">
         <v>1</v>
       </c>
-      <c r="AD10">
-        <v>1</v>
-      </c>
-      <c r="AE10">
-        <v>1</v>
-      </c>
-      <c r="AI10">
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="Y11">
-        <v>1</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AI11">
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+      <c r="AV11">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>10</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-      <c r="AI12">
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AV12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13">
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
         <v>7</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="AD13">
-        <v>2</v>
-      </c>
-      <c r="AI13">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <v>2</v>
+      </c>
+      <c r="AV13">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1653,66 +1767,66 @@
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>7</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
-      <c r="U14">
-        <v>2</v>
-      </c>
-      <c r="W14">
-        <v>2</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-      <c r="AI14">
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>2</v>
+      </c>
+      <c r="AF14">
+        <v>2</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AV14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>15</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
+      <c r="O15">
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>2</v>
-      </c>
-      <c r="Y15">
-        <v>2</v>
-      </c>
-      <c r="AA15">
-        <v>1</v>
-      </c>
-      <c r="AD15">
-        <v>2</v>
-      </c>
-      <c r="AI15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>2</v>
+      </c>
+      <c r="AH15">
+        <v>2</v>
+      </c>
+      <c r="AJ15">
+        <v>1</v>
+      </c>
+      <c r="AO15">
+        <v>2</v>
+      </c>
+      <c r="AV15">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -1722,271 +1836,501 @@
       <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="I16">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="L16">
         <v>16</v>
       </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
       <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="U16">
         <v>6</v>
       </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="U16">
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
         <v>4</v>
       </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>2</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Z16">
-        <v>1</v>
-      </c>
-      <c r="AB16">
-        <v>1</v>
-      </c>
-      <c r="AC16">
-        <v>3</v>
-      </c>
       <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>2</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AN16">
+        <v>3</v>
+      </c>
+      <c r="AO16">
         <v>4</v>
       </c>
-      <c r="AE16">
-        <v>1</v>
-      </c>
-      <c r="AG16">
-        <v>1</v>
-      </c>
-      <c r="AH16">
-        <v>2</v>
-      </c>
-      <c r="AI16">
-        <f>SUM(B16:AH16)</f>
+      <c r="AP16">
+        <v>1</v>
+      </c>
+      <c r="AR16">
+        <v>1</v>
+      </c>
+      <c r="AS16">
+        <v>2</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="I17">
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="L17">
         <v>23</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
       <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
         <v>7</v>
       </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="T17">
+      <c r="R17">
         <v>1</v>
       </c>
       <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
         <v>4</v>
       </c>
-      <c r="V17">
-        <v>2</v>
-      </c>
-      <c r="W17">
+      <c r="AD17">
+        <v>2</v>
+      </c>
+      <c r="AF17">
         <v>7</v>
       </c>
-      <c r="Y17">
-        <v>3</v>
-      </c>
-      <c r="Z17">
+      <c r="AH17">
+        <v>3</v>
+      </c>
+      <c r="AI17">
         <v>10</v>
       </c>
-      <c r="AC17">
-        <v>2</v>
-      </c>
-      <c r="AD17">
+      <c r="AN17">
+        <v>2</v>
+      </c>
+      <c r="AO17">
         <v>5</v>
       </c>
-      <c r="AI17">
-        <f>SUM(B17:AH17)</f>
+      <c r="AV17">
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f>SUM(B2:B17)</f>
-        <v>1</v>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43912</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:AI18" si="1">SUM(C2:C17)</f>
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>13</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>11</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>2</v>
+      </c>
+      <c r="AC18">
+        <v>5</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
         <v>4</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="1"/>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>2</v>
+      </c>
+      <c r="AJ18">
+        <v>4</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
+      </c>
+      <c r="AN18">
+        <v>2</v>
+      </c>
+      <c r="AO18">
         <v>8</v>
       </c>
-      <c r="R18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="1"/>
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+      <c r="AS18">
+        <v>1</v>
+      </c>
+      <c r="AU18">
+        <v>1</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43913</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>24</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="U19">
+        <v>7</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>2</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>5</v>
+      </c>
+      <c r="AD19">
         <v>4</v>
       </c>
-      <c r="T18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="1"/>
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>5</v>
+      </c>
+      <c r="AG19">
+        <v>2</v>
+      </c>
+      <c r="AH19">
+        <v>5</v>
+      </c>
+      <c r="AI19">
         <v>4</v>
       </c>
-      <c r="W18">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="X18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <f t="shared" si="1"/>
+      <c r="AJ19">
+        <v>2</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AM19">
+        <v>1</v>
+      </c>
+      <c r="AN19">
+        <v>2</v>
+      </c>
+      <c r="AO19">
+        <v>5</v>
+      </c>
+      <c r="AS19">
+        <v>2</v>
+      </c>
+      <c r="AT19">
+        <v>1</v>
+      </c>
+      <c r="AU19">
+        <v>1</v>
+      </c>
+      <c r="AV19">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" ref="B20" si="1">SUM(B2:B19)</f>
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20" si="2">SUM(C2:C19)</f>
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20" si="3">SUM(D2:D19)</f>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="4">SUM(E2:E19)</f>
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20" si="5">SUM(F2:F19)</f>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20" si="6">SUM(G2:G19)</f>
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20" si="7">SUM(H2:H19)</f>
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20" si="8">SUM(I2:I19)</f>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ref="J20" si="9">SUM(J2:J19)</f>
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ref="K20" si="10">SUM(K2:K19)</f>
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20" si="11">SUM(L2:L19)</f>
+        <v>149</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ref="M20" si="12">SUM(M2:M19)</f>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ref="N20" si="13">SUM(N2:N19)</f>
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ref="O20" si="14">SUM(O2:O19)</f>
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ref="P20" si="15">SUM(P2:P19)</f>
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ref="Q20" si="16">SUM(Q2:Q19)</f>
+        <v>44</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ref="R20" si="17">SUM(R2:R19)</f>
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <f t="shared" ref="S20" si="18">SUM(S2:S19)</f>
+        <v>2</v>
+      </c>
+      <c r="T20">
+        <f t="shared" ref="T20" si="19">SUM(T2:T19)</f>
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <f t="shared" ref="U20" si="20">SUM(U2:U19)</f>
+        <v>26</v>
+      </c>
+      <c r="V20">
+        <f t="shared" ref="V20" si="21">SUM(V2:V19)</f>
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <f t="shared" ref="W20" si="22">SUM(W2:W19)</f>
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <f t="shared" ref="X20" si="23">SUM(X2:X19)</f>
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" ref="Y20" si="24">SUM(Y2:Y19)</f>
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" ref="Z20" si="25">SUM(Z2:Z19)</f>
+        <v>8</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" ref="AA20" si="26">SUM(AA2:AA19)</f>
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" ref="AB20" si="27">SUM(AB2:AB19)</f>
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" ref="AC20" si="28">SUM(AC2:AC19)</f>
+        <v>24</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" ref="AD20" si="29">SUM(AD2:AD19)</f>
         <v>9</v>
       </c>
-      <c r="Z18">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="AA18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AC18">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AD18">
-        <f t="shared" si="1"/>
+      <c r="AE20">
+        <f t="shared" ref="AE20" si="30">SUM(AE2:AE19)</f>
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" ref="AF20" si="31">SUM(AF2:AF19)</f>
+        <v>23</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" ref="AG20" si="32">SUM(AG2:AG19)</f>
+        <v>3</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" ref="AH20" si="33">SUM(AH2:AH19)</f>
         <v>15</v>
       </c>
-      <c r="AE18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AF18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AG18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AH18">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AI18">
-        <f t="shared" si="1"/>
-        <v>247</v>
-      </c>
+      <c r="AI20">
+        <f t="shared" ref="AI20" si="34">SUM(AI2:AI19)</f>
+        <v>17</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" ref="AJ20" si="35">SUM(AJ2:AJ19)</f>
+        <v>7</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" ref="AK20" si="36">SUM(AK2:AK19)</f>
+        <v>2</v>
+      </c>
+      <c r="AL20">
+        <f t="shared" ref="AL20" si="37">SUM(AL2:AL19)</f>
+        <v>1</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" ref="AM20" si="38">SUM(AM2:AM19)</f>
+        <v>1</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" ref="AN20" si="39">SUM(AN2:AN19)</f>
+        <v>12</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" ref="AO20" si="40">SUM(AO2:AO19)</f>
+        <v>28</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" ref="AP20" si="41">SUM(AP2:AP19)</f>
+        <v>3</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" ref="AQ20" si="42">SUM(AQ2:AQ19)</f>
+        <v>2</v>
+      </c>
+      <c r="AR20">
+        <f t="shared" ref="AR20" si="43">SUM(AR2:AR19)</f>
+        <v>1</v>
+      </c>
+      <c r="AS20">
+        <f t="shared" ref="AS20" si="44">SUM(AS2:AS19)</f>
+        <v>5</v>
+      </c>
+      <c r="AT20">
+        <f t="shared" ref="AT20" si="45">SUM(AT2:AT19)</f>
+        <v>1</v>
+      </c>
+      <c r="AU20">
+        <f t="shared" ref="AU20:AV20" si="46">SUM(AU2:AU19)</f>
+        <v>2</v>
+      </c>
+      <c r="AV20">
+        <f t="shared" si="46"/>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +2338,7 @@
     <col min="1" max="1" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2002,22 +2346,28 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43910</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
-        <f>SUM(B2:D2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>SUM(B2:F2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43911</v>
       </c>
@@ -2027,27 +2377,59 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <f>SUM(B3:D3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>SUM(B2:B3)</f>
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:D4" si="0">SUM(C2:C3)</f>
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="G3">
+        <f>SUM(B3:F3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43912</v>
+      </c>
+      <c r="G4">
+        <f>SUM(B4:F4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43913</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f>SUM(B5:F5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:F6" si="0">SUM(C2:C5)</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f>SUM(E2:E3)</f>
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>SUM(B6:F6)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -4169,7 +4551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13:V13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update fit_logistic and Update data for 3/25
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Negative PUIs</t>
   </si>
@@ -225,6 +225,21 @@
   </si>
   <si>
     <t>Madison</t>
+  </si>
+  <si>
+    <t>ICU admissions</t>
+  </si>
+  <si>
+    <t>Age range</t>
+  </si>
+  <si>
+    <t>&lt;1 - 94</t>
+  </si>
+  <si>
+    <t>Median age</t>
+  </si>
+  <si>
+    <t>Male percent</t>
   </si>
 </sst>
 </file>
@@ -722,7 +737,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -733,6 +748,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1054,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1083,7 @@
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1086,8 +1102,20 @@
       <c r="G1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43896</v>
       </c>
@@ -1104,7 +1132,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43897</v>
       </c>
@@ -1121,7 +1149,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43898</v>
       </c>
@@ -1138,7 +1166,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -1155,7 +1183,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43900</v>
       </c>
@@ -1175,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43901</v>
       </c>
@@ -1192,7 +1220,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -1209,7 +1237,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43903</v>
       </c>
@@ -1226,7 +1254,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43904</v>
       </c>
@@ -1243,7 +1271,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43905</v>
       </c>
@@ -1260,7 +1288,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43906</v>
       </c>
@@ -1280,7 +1308,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43907</v>
       </c>
@@ -1294,7 +1322,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43908</v>
       </c>
@@ -1308,7 +1336,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43909</v>
       </c>
@@ -1322,7 +1350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43910</v>
       </c>
@@ -1336,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43911</v>
       </c>
@@ -1350,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43912</v>
       </c>
@@ -1364,7 +1392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43913</v>
       </c>
@@ -1376,6 +1404,46 @@
       </c>
       <c r="G19">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B20">
+        <v>564</v>
+      </c>
+      <c r="E20">
+        <v>145</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B21">
+        <v>704</v>
+      </c>
+      <c r="E21">
+        <v>182</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21">
+        <v>51</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>